<commit_message>
People Keep Taking the Colors Survey
</commit_message>
<xml_diff>
--- a/Colors Email Merge/21-22 T3 True Colors(TM) Communication Survey ANALYZER.xlsx
+++ b/Colors Email Merge/21-22 T3 True Colors(TM) Communication Survey ANALYZER.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JohnWeis\Documents\GitHub\Misc\Colors Email Merge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E4495FDE-3A43-4922-9E0E-FF76BF864BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E086FE04-2EF6-43E6-8E49-7927FF585FA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38370" yWindow="-14520" windowWidth="18240" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-14520" windowWidth="18240" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INSTRUCTIONS" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="234">
   <si>
     <t>1.</t>
   </si>
@@ -681,6 +681,72 @@
   </si>
   <si>
     <t>Lupita Cortes</t>
+  </si>
+  <si>
+    <t>gilbert530@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Gilbert Mendoza</t>
+  </si>
+  <si>
+    <t>ayden705@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Ayden Eves</t>
+  </si>
+  <si>
+    <t>yizel309@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Yizel Zayas</t>
+  </si>
+  <si>
+    <t>lucia276@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Lucia Robles</t>
+  </si>
+  <si>
+    <t>wyatt381@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Wyatt Edwards</t>
+  </si>
+  <si>
+    <t>sayda106@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Sayda Meras Alvarez</t>
+  </si>
+  <si>
+    <t>andres902@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Andres Cabezas</t>
+  </si>
+  <si>
+    <t>cezar960@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Cezar Sanchez Penaloza</t>
+  </si>
+  <si>
+    <t>celene340@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Celene Ortiz Jimenez</t>
+  </si>
+  <si>
+    <t>tonkra001@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Tonkra Phomtanaphun</t>
+  </si>
+  <si>
+    <t>bennett352@students.psd1.org</t>
+  </si>
+  <si>
+    <t>Bennett McDonald</t>
   </si>
 </sst>
 </file>
@@ -728,11 +794,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -830,8 +900,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Y53" totalsRowShown="0">
-  <autoFilter ref="A1:Y53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:Y67" totalsRowShown="0">
+  <autoFilter ref="A1:Y67" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="24"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="23"/>
@@ -1249,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y53"/>
+  <dimension ref="A1:Y67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5599,6 +5669,1154 @@
       <c r="Y53" s="5">
         <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
         <v>5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>196</v>
+      </c>
+      <c r="B54" s="6">
+        <v>44636.922256944403</v>
+      </c>
+      <c r="C54" s="6">
+        <v>44636.923379629603</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="J54" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K54" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L54" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="M54" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="N54" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O54" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P54" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q54" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R54" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="S54" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="T54" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="U54" s="7">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H54,COLORLOOKUP,2),VLOOKUP(I54,COLORLOOKUP,2),VLOOKUP(J54,COLORLOOKUP,2),VLOOKUP(K54,COLORLOOKUP,2),VLOOKUP(L54,COLORLOOKUP,2),VLOOKUP(M54,COLORLOOKUP,2),VLOOKUP(N54,COLORLOOKUP,2),VLOOKUP(O54,COLORLOOKUP,2),VLOOKUP(P54,COLORLOOKUP,2),VLOOKUP(Q54,COLORLOOKUP,2),VLOOKUP(R54,COLORLOOKUP,2),VLOOKUP(S54,COLORLOOKUP,2),VLOOKUP(T54,COLORLOOKUP,2))</f>
+        <v>3040206</v>
+      </c>
+      <c r="V54" s="7">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="W54" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>4</v>
+      </c>
+      <c r="X54" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>2</v>
+      </c>
+      <c r="Y54" s="7">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>197</v>
+      </c>
+      <c r="B55" s="6">
+        <v>44637.372731481497</v>
+      </c>
+      <c r="C55" s="6">
+        <v>44637.373263888898</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="J55" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="K55" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L55" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M55" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="N55" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="O55" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="P55" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="T55" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U55" s="7">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H55,COLORLOOKUP,2),VLOOKUP(I55,COLORLOOKUP,2),VLOOKUP(J55,COLORLOOKUP,2),VLOOKUP(K55,COLORLOOKUP,2),VLOOKUP(L55,COLORLOOKUP,2),VLOOKUP(M55,COLORLOOKUP,2),VLOOKUP(N55,COLORLOOKUP,2),VLOOKUP(O55,COLORLOOKUP,2),VLOOKUP(P55,COLORLOOKUP,2),VLOOKUP(Q55,COLORLOOKUP,2),VLOOKUP(R55,COLORLOOKUP,2),VLOOKUP(S55,COLORLOOKUP,2),VLOOKUP(T55,COLORLOOKUP,2))</f>
+        <v>5020305</v>
+      </c>
+      <c r="V55" s="7">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>5</v>
+      </c>
+      <c r="W55" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>2</v>
+      </c>
+      <c r="X55" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="Y55" s="7">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>198</v>
+      </c>
+      <c r="B56" s="6">
+        <v>44637.418356481503</v>
+      </c>
+      <c r="C56" s="6">
+        <v>44637.4198032407</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J56" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="K56" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="L56" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="M56" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="N56" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="O56" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="P56" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q56" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="R56" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="S56" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="T56" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="U56" s="7">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H56,COLORLOOKUP,2),VLOOKUP(I56,COLORLOOKUP,2),VLOOKUP(J56,COLORLOOKUP,2),VLOOKUP(K56,COLORLOOKUP,2),VLOOKUP(L56,COLORLOOKUP,2),VLOOKUP(M56,COLORLOOKUP,2),VLOOKUP(N56,COLORLOOKUP,2),VLOOKUP(O56,COLORLOOKUP,2),VLOOKUP(P56,COLORLOOKUP,2),VLOOKUP(Q56,COLORLOOKUP,2),VLOOKUP(R56,COLORLOOKUP,2),VLOOKUP(S56,COLORLOOKUP,2),VLOOKUP(T56,COLORLOOKUP,2))</f>
+        <v>1000311</v>
+      </c>
+      <c r="V56" s="7">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>1</v>
+      </c>
+      <c r="W56" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>0</v>
+      </c>
+      <c r="X56" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="Y56" s="7">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>199</v>
+      </c>
+      <c r="B57" s="6">
+        <v>44637.435902777797</v>
+      </c>
+      <c r="C57" s="6">
+        <v>44637.4368287037</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="J57" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K57" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L57" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="M57" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="N57" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O57" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="P57" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q57" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="T57" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="U57" s="7">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H57,COLORLOOKUP,2),VLOOKUP(I57,COLORLOOKUP,2),VLOOKUP(J57,COLORLOOKUP,2),VLOOKUP(K57,COLORLOOKUP,2),VLOOKUP(L57,COLORLOOKUP,2),VLOOKUP(M57,COLORLOOKUP,2),VLOOKUP(N57,COLORLOOKUP,2),VLOOKUP(O57,COLORLOOKUP,2),VLOOKUP(P57,COLORLOOKUP,2),VLOOKUP(Q57,COLORLOOKUP,2),VLOOKUP(R57,COLORLOOKUP,2),VLOOKUP(S57,COLORLOOKUP,2),VLOOKUP(T57,COLORLOOKUP,2))</f>
+        <v>8010501</v>
+      </c>
+      <c r="V57" s="7">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>8</v>
+      </c>
+      <c r="W57" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>1</v>
+      </c>
+      <c r="X57" s="7">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>5</v>
+      </c>
+      <c r="Y57" s="7">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>200</v>
+      </c>
+      <c r="B58" s="8">
+        <v>44637.447337963</v>
+      </c>
+      <c r="C58" s="8">
+        <v>44637.448634259301</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E58" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="F58" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G58" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H58" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I58" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J58" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K58" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L58" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M58" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N58" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O58" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="P58" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q58" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="R58" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S58" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T58" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="U58" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H58,COLORLOOKUP,2),VLOOKUP(I58,COLORLOOKUP,2),VLOOKUP(J58,COLORLOOKUP,2),VLOOKUP(K58,COLORLOOKUP,2),VLOOKUP(L58,COLORLOOKUP,2),VLOOKUP(M58,COLORLOOKUP,2),VLOOKUP(N58,COLORLOOKUP,2),VLOOKUP(O58,COLORLOOKUP,2),VLOOKUP(P58,COLORLOOKUP,2),VLOOKUP(Q58,COLORLOOKUP,2),VLOOKUP(R58,COLORLOOKUP,2),VLOOKUP(S58,COLORLOOKUP,2),VLOOKUP(T58,COLORLOOKUP,2))</f>
+        <v>12000102</v>
+      </c>
+      <c r="V58" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>12</v>
+      </c>
+      <c r="W58" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>0</v>
+      </c>
+      <c r="X58" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>1</v>
+      </c>
+      <c r="Y58" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>201</v>
+      </c>
+      <c r="B59" s="8">
+        <v>44637.448449074102</v>
+      </c>
+      <c r="C59" s="8">
+        <v>44637.450115740699</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E59" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="F59" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G59" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H59" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I59" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="J59" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K59" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L59" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="M59" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N59" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="O59" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="P59" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q59" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="R59" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S59" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="T59" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="U59" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H59,COLORLOOKUP,2),VLOOKUP(I59,COLORLOOKUP,2),VLOOKUP(J59,COLORLOOKUP,2),VLOOKUP(K59,COLORLOOKUP,2),VLOOKUP(L59,COLORLOOKUP,2),VLOOKUP(M59,COLORLOOKUP,2),VLOOKUP(N59,COLORLOOKUP,2),VLOOKUP(O59,COLORLOOKUP,2),VLOOKUP(P59,COLORLOOKUP,2),VLOOKUP(Q59,COLORLOOKUP,2),VLOOKUP(R59,COLORLOOKUP,2),VLOOKUP(S59,COLORLOOKUP,2),VLOOKUP(T59,COLORLOOKUP,2))</f>
+        <v>2070204</v>
+      </c>
+      <c r="V59" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>2</v>
+      </c>
+      <c r="W59" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>7</v>
+      </c>
+      <c r="X59" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>2</v>
+      </c>
+      <c r="Y59" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>202</v>
+      </c>
+      <c r="B60" s="8">
+        <v>44637.479375000003</v>
+      </c>
+      <c r="C60" s="8">
+        <v>44637.479884259301</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E60" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="F60" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J60" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K60" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L60" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M60" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N60" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O60" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="P60" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q60" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="R60" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S60" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T60" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="U60" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H60,COLORLOOKUP,2),VLOOKUP(I60,COLORLOOKUP,2),VLOOKUP(J60,COLORLOOKUP,2),VLOOKUP(K60,COLORLOOKUP,2),VLOOKUP(L60,COLORLOOKUP,2),VLOOKUP(M60,COLORLOOKUP,2),VLOOKUP(N60,COLORLOOKUP,2),VLOOKUP(O60,COLORLOOKUP,2),VLOOKUP(P60,COLORLOOKUP,2),VLOOKUP(Q60,COLORLOOKUP,2),VLOOKUP(R60,COLORLOOKUP,2),VLOOKUP(S60,COLORLOOKUP,2),VLOOKUP(T60,COLORLOOKUP,2))</f>
+        <v>6030501</v>
+      </c>
+      <c r="V60" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>6</v>
+      </c>
+      <c r="W60" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="X60" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>5</v>
+      </c>
+      <c r="Y60" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>203</v>
+      </c>
+      <c r="B61" s="8">
+        <v>44637.494918981502</v>
+      </c>
+      <c r="C61" s="8">
+        <v>44637.496296296304</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E61" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="F61" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="J61" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K61" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L61" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M61" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N61" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="O61" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P61" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q61" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S61" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="T61" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="U61" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H61,COLORLOOKUP,2),VLOOKUP(I61,COLORLOOKUP,2),VLOOKUP(J61,COLORLOOKUP,2),VLOOKUP(K61,COLORLOOKUP,2),VLOOKUP(L61,COLORLOOKUP,2),VLOOKUP(M61,COLORLOOKUP,2),VLOOKUP(N61,COLORLOOKUP,2),VLOOKUP(O61,COLORLOOKUP,2),VLOOKUP(P61,COLORLOOKUP,2),VLOOKUP(Q61,COLORLOOKUP,2),VLOOKUP(R61,COLORLOOKUP,2),VLOOKUP(S61,COLORLOOKUP,2),VLOOKUP(T61,COLORLOOKUP,2))</f>
+        <v>3030603</v>
+      </c>
+      <c r="V61" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="W61" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="X61" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>6</v>
+      </c>
+      <c r="Y61" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>204</v>
+      </c>
+      <c r="B62" s="8">
+        <v>44637.516909722202</v>
+      </c>
+      <c r="C62" s="8">
+        <v>44637.518148148098</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E62" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="F62" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G62" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H62" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I62" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J62" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K62" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L62" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M62" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="N62" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O62" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P62" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q62" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="R62" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S62" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="T62" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="U62" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H62,COLORLOOKUP,2),VLOOKUP(I62,COLORLOOKUP,2),VLOOKUP(J62,COLORLOOKUP,2),VLOOKUP(K62,COLORLOOKUP,2),VLOOKUP(L62,COLORLOOKUP,2),VLOOKUP(M62,COLORLOOKUP,2),VLOOKUP(N62,COLORLOOKUP,2),VLOOKUP(O62,COLORLOOKUP,2),VLOOKUP(P62,COLORLOOKUP,2),VLOOKUP(Q62,COLORLOOKUP,2),VLOOKUP(R62,COLORLOOKUP,2),VLOOKUP(S62,COLORLOOKUP,2),VLOOKUP(T62,COLORLOOKUP,2))</f>
+        <v>5030007</v>
+      </c>
+      <c r="V62" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>5</v>
+      </c>
+      <c r="W62" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="X62" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y62" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>205</v>
+      </c>
+      <c r="B63" s="8">
+        <v>44637.527974536999</v>
+      </c>
+      <c r="C63" s="8">
+        <v>44637.529166666704</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="E63" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G63" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="H63" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I63" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J63" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K63" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L63" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M63" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N63" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O63" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P63" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q63" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="R63" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S63" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T63" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="U63" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H63,COLORLOOKUP,2),VLOOKUP(I63,COLORLOOKUP,2),VLOOKUP(J63,COLORLOOKUP,2),VLOOKUP(K63,COLORLOOKUP,2),VLOOKUP(L63,COLORLOOKUP,2),VLOOKUP(M63,COLORLOOKUP,2),VLOOKUP(N63,COLORLOOKUP,2),VLOOKUP(O63,COLORLOOKUP,2),VLOOKUP(P63,COLORLOOKUP,2),VLOOKUP(Q63,COLORLOOKUP,2),VLOOKUP(R63,COLORLOOKUP,2),VLOOKUP(S63,COLORLOOKUP,2),VLOOKUP(T63,COLORLOOKUP,2))</f>
+        <v>4020405</v>
+      </c>
+      <c r="V63" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>4</v>
+      </c>
+      <c r="W63" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>2</v>
+      </c>
+      <c r="X63" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>4</v>
+      </c>
+      <c r="Y63" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>206</v>
+      </c>
+      <c r="B64" s="8">
+        <v>44637.537233796298</v>
+      </c>
+      <c r="C64" s="8">
+        <v>44637.538449074098</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="E64" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="G64" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H64" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I64" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J64" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K64" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L64" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M64" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="N64" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="O64" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P64" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q64" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="R64" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="S64" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="T64" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="U64" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H64,COLORLOOKUP,2),VLOOKUP(I64,COLORLOOKUP,2),VLOOKUP(J64,COLORLOOKUP,2),VLOOKUP(K64,COLORLOOKUP,2),VLOOKUP(L64,COLORLOOKUP,2),VLOOKUP(M64,COLORLOOKUP,2),VLOOKUP(N64,COLORLOOKUP,2),VLOOKUP(O64,COLORLOOKUP,2),VLOOKUP(P64,COLORLOOKUP,2),VLOOKUP(Q64,COLORLOOKUP,2),VLOOKUP(R64,COLORLOOKUP,2),VLOOKUP(S64,COLORLOOKUP,2),VLOOKUP(T64,COLORLOOKUP,2))</f>
+        <v>3040008</v>
+      </c>
+      <c r="V64" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="W64" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>4</v>
+      </c>
+      <c r="X64" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>0</v>
+      </c>
+      <c r="Y64" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="65" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>207</v>
+      </c>
+      <c r="B65" s="8">
+        <v>44637.5374421296</v>
+      </c>
+      <c r="C65" s="8">
+        <v>44637.539074074099</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="E65" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="F65" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G65" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H65" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I65" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="J65" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K65" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="L65" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M65" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N65" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O65" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P65" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q65" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R65" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S65" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T65" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="U65" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H65,COLORLOOKUP,2),VLOOKUP(I65,COLORLOOKUP,2),VLOOKUP(J65,COLORLOOKUP,2),VLOOKUP(K65,COLORLOOKUP,2),VLOOKUP(L65,COLORLOOKUP,2),VLOOKUP(M65,COLORLOOKUP,2),VLOOKUP(N65,COLORLOOKUP,2),VLOOKUP(O65,COLORLOOKUP,2),VLOOKUP(P65,COLORLOOKUP,2),VLOOKUP(Q65,COLORLOOKUP,2),VLOOKUP(R65,COLORLOOKUP,2),VLOOKUP(S65,COLORLOOKUP,2),VLOOKUP(T65,COLORLOOKUP,2))</f>
+        <v>5050302</v>
+      </c>
+      <c r="V65" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>5</v>
+      </c>
+      <c r="W65" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>5</v>
+      </c>
+      <c r="X65" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="Y65" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
+        <v>208</v>
+      </c>
+      <c r="B66" s="8">
+        <v>44637.538240740701</v>
+      </c>
+      <c r="C66" s="8">
+        <v>44637.540509259299</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="E66" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="G66" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="H66" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I66" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J66" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K66" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="L66" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="M66" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N66" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O66" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="P66" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q66" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="R66" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S66" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="T66" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="U66" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H66,COLORLOOKUP,2),VLOOKUP(I66,COLORLOOKUP,2),VLOOKUP(J66,COLORLOOKUP,2),VLOOKUP(K66,COLORLOOKUP,2),VLOOKUP(L66,COLORLOOKUP,2),VLOOKUP(M66,COLORLOOKUP,2),VLOOKUP(N66,COLORLOOKUP,2),VLOOKUP(O66,COLORLOOKUP,2),VLOOKUP(P66,COLORLOOKUP,2),VLOOKUP(Q66,COLORLOOKUP,2),VLOOKUP(R66,COLORLOOKUP,2),VLOOKUP(S66,COLORLOOKUP,2),VLOOKUP(T66,COLORLOOKUP,2))</f>
+        <v>6030204</v>
+      </c>
+      <c r="V66" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>6</v>
+      </c>
+      <c r="W66" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>3</v>
+      </c>
+      <c r="X66" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>2</v>
+      </c>
+      <c r="Y66" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
+        <v>209</v>
+      </c>
+      <c r="B67" s="8">
+        <v>44637.541076388901</v>
+      </c>
+      <c r="C67" s="8">
+        <v>44637.542268518497</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="E67" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G67" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H67" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I67" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="J67" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="K67" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L67" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M67" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N67" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="O67" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="P67" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q67" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R67" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S67" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="T67" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="U67" s="9">
+        <f>SUM(VLOOKUP(Table1[[#This Row],[Which word do you like the most?]],COLORLOOKUP,2),VLOOKUP(Table1[[#This Row],[Which word do you like the most?2]],COLORLOOKUP,2),VLOOKUP(H67,COLORLOOKUP,2),VLOOKUP(I67,COLORLOOKUP,2),VLOOKUP(J67,COLORLOOKUP,2),VLOOKUP(K67,COLORLOOKUP,2),VLOOKUP(L67,COLORLOOKUP,2),VLOOKUP(M67,COLORLOOKUP,2),VLOOKUP(N67,COLORLOOKUP,2),VLOOKUP(O67,COLORLOOKUP,2),VLOOKUP(P67,COLORLOOKUP,2),VLOOKUP(Q67,COLORLOOKUP,2),VLOOKUP(R67,COLORLOOKUP,2),VLOOKUP(S67,COLORLOOKUP,2),VLOOKUP(T67,COLORLOOKUP,2))</f>
+        <v>5060202</v>
+      </c>
+      <c r="V67" s="9">
+        <f>INT(Table1[[#This Row],[Total Score]]/ORANGEVALUE)</f>
+        <v>5</v>
+      </c>
+      <c r="W67" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE)/GOLDVALUE)</f>
+        <v>6</v>
+      </c>
+      <c r="X67" s="9">
+        <f>INT((Table1[[#This Row],[Total Score]]-Table1[[#This Row],[Orange]]*ORANGEVALUE-Table1[[#This Row],[Gold]]*GOLDVALUE)/BLUEVALUE)</f>
+        <v>2</v>
+      </c>
+      <c r="Y67" s="9">
+        <f>MOD(Table1[[#This Row],[Total Score]],BLUEVALUE)</f>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>